<commit_message>
IN-999 Add Logtime to mapping for client_notes
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82F487E-AF88-1F43-902C-4AB6FD7391DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC274306-3ECF-034C-8B7B-5655BA4C1EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="6120" windowWidth="27440" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30380" yWindow="6880" windowWidth="27440" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="96">
   <si>
     <t>table_name</t>
   </si>
@@ -131,9 +131,6 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>Logdate</t>
-  </si>
-  <si>
     <t>createdbyuser_id</t>
   </si>
   <si>
@@ -309,6 +306,13 @@
   </si>
   <si>
     <t>EVENT_CREATED</t>
+  </si>
+  <si>
+    <t>Logdate
+Logtime</t>
+  </si>
+  <si>
+    <t>convert_to_timestamp</t>
   </si>
 </sst>
 </file>
@@ -445,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -475,6 +479,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,76 +708,76 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>80</v>
       </c>
       <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
         <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>82</v>
-      </c>
       <c r="F3" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -784,7 +791,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -887,7 +894,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -896,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>27</v>
@@ -920,7 +927,7 @@
       </c>
       <c r="M4" s="2"/>
       <c r="O4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -931,7 +938,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>21</v>
@@ -955,7 +962,7 @@
         <v>27</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -984,10 +991,10 @@
         <v>30</v>
       </c>
       <c r="M6" t="s">
+        <v>84</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1010,7 +1017,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="31" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1032,11 +1039,14 @@
       <c r="I8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>35</v>
+      <c r="J8" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" t="s">
+        <v>95</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1047,7 +1057,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -1056,16 +1066,16 @@
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M9" s="2">
         <v>2</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1076,7 +1086,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>21</v>
@@ -1091,10 +1101,10 @@
         <v>25</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="14" x14ac:dyDescent="0.15">
@@ -2614,7 +2624,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>19</v>
@@ -2623,7 +2633,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>27</v>
@@ -2647,7 +2657,7 @@
       </c>
       <c r="M4" s="15"/>
       <c r="O4" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2658,7 +2668,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>21</v>
@@ -2667,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>24</v>
@@ -2682,7 +2692,7 @@
         <v>27</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2702,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>29</v>
@@ -2711,7 +2721,7 @@
         <v>30</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2752,16 +2762,16 @@
         <v>0</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>34</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2772,7 +2782,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>19</v>
@@ -2781,17 +2791,17 @@
         <v>0</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="15"/>
       <c r="M9" s="15">
         <v>2</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2802,7 +2812,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>21</v>
@@ -2811,16 +2821,16 @@
         <v>0</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>25</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4251,160 +4261,160 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -5867,160 +5877,160 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
IN-999 Combine "Logdate" and "Logtime" to set a "createdtime" on client notes (#436)
* IN-999 Add Logtime to mapping for client_notes

* IN-999 Add convert_to_timestamp transformation

* IN-999 Add unit tests for convert_to_timestamp transformation

* IN-999 Change validation overrides from partial to full overrides

* IN-999 Update validation for createdtime on client notes; Re-enable address_lines validation

* IN-999 Use a timestamp(0) data type for all date/time columns in the transform schema

* IN-999 Add a default_date argument to validation function
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82F487E-AF88-1F43-902C-4AB6FD7391DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC274306-3ECF-034C-8B7B-5655BA4C1EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="6120" windowWidth="27440" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30380" yWindow="6880" windowWidth="27440" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="96">
   <si>
     <t>table_name</t>
   </si>
@@ -131,9 +131,6 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>Logdate</t>
-  </si>
-  <si>
     <t>createdbyuser_id</t>
   </si>
   <si>
@@ -309,6 +306,13 @@
   </si>
   <si>
     <t>EVENT_CREATED</t>
+  </si>
+  <si>
+    <t>Logdate
+Logtime</t>
+  </si>
+  <si>
+    <t>convert_to_timestamp</t>
   </si>
 </sst>
 </file>
@@ -445,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -475,6 +479,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,76 +708,76 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>80</v>
       </c>
       <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
         <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>82</v>
-      </c>
       <c r="F3" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -784,7 +791,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -887,7 +894,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -896,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>27</v>
@@ -920,7 +927,7 @@
       </c>
       <c r="M4" s="2"/>
       <c r="O4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -931,7 +938,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>21</v>
@@ -955,7 +962,7 @@
         <v>27</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -984,10 +991,10 @@
         <v>30</v>
       </c>
       <c r="M6" t="s">
+        <v>84</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1010,7 +1017,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="31" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1032,11 +1039,14 @@
       <c r="I8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>35</v>
+      <c r="J8" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" t="s">
+        <v>95</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1047,7 +1057,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -1056,16 +1066,16 @@
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M9" s="2">
         <v>2</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1076,7 +1086,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>21</v>
@@ -1091,10 +1101,10 @@
         <v>25</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="14" x14ac:dyDescent="0.15">
@@ -2614,7 +2624,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>19</v>
@@ -2623,7 +2633,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>27</v>
@@ -2647,7 +2657,7 @@
       </c>
       <c r="M4" s="15"/>
       <c r="O4" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2658,7 +2668,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>21</v>
@@ -2667,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>24</v>
@@ -2682,7 +2692,7 @@
         <v>27</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2702,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>29</v>
@@ -2711,7 +2721,7 @@
         <v>30</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2752,16 +2762,16 @@
         <v>0</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>34</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2772,7 +2782,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>19</v>
@@ -2781,17 +2791,17 @@
         <v>0</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="15"/>
       <c r="M9" s="15">
         <v>2</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2802,7 +2812,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>21</v>
@@ -2811,16 +2821,16 @@
         <v>0</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>25</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4251,160 +4261,160 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
@@ -5867,160 +5877,160 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Trim note description, also fix createdtime for deputy notes
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuahawxwell/dev/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC274306-3ECF-034C-8B7B-5655BA4C1EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79C2BE3-66C3-EB4D-B506-1827A668B1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30380" yWindow="6880" windowWidth="27440" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30380" yWindow="4060" windowWidth="27440" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="96">
   <si>
     <t>table_name</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>DEPUTY_REMARKS</t>
-  </si>
-  <si>
-    <t>Log Date</t>
   </si>
   <si>
     <t>Deputy No</t>
@@ -313,6 +310,10 @@
   </si>
   <si>
     <t>convert_to_timestamp</t>
+  </si>
+  <si>
+    <t>Log Date
+Log Time</t>
   </si>
 </sst>
 </file>
@@ -449,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -480,6 +481,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -773,11 +777,11 @@
         <v>81</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -789,9 +793,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1040,10 +1044,10 @@
         <v>34</v>
       </c>
       <c r="J8" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" t="s">
         <v>94</v>
-      </c>
-      <c r="K8" t="s">
-        <v>95</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>85</v>
@@ -2518,9 +2522,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEA7712-2DD9-FE43-BF40-300AEE11EF42}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2724,7 +2728,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>16</v>
       </c>
@@ -2745,7 +2749,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="31" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>16</v>
       </c>
@@ -2767,8 +2771,11 @@
       <c r="I8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="14" t="s">
-        <v>90</v>
+      <c r="J8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="K8" t="s">
+        <v>94</v>
       </c>
       <c r="O8" s="14" t="s">
         <v>85</v>
@@ -5898,7 +5905,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5910,7 +5917,7 @@
         <v>47</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5922,7 +5929,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5934,7 +5941,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5946,7 +5953,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5958,7 +5965,7 @@
         <v>55</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5970,7 +5977,7 @@
         <v>57</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5982,7 +5989,7 @@
         <v>60</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5994,7 +6001,7 @@
         <v>62</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6006,7 +6013,7 @@
         <v>64</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6018,7 +6025,7 @@
         <v>66</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -6030,7 +6037,7 @@
         <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
IN-1030 update note subtypes
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuahawxwell/dev/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79C2BE3-66C3-EB4D-B506-1827A668B1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C9220-D9CD-2E48-8394-4D1A5D430114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30380" yWindow="4060" windowWidth="27440" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15420" yWindow="5940" windowWidth="35400" windowHeight="22480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="108">
   <si>
     <t>table_name</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>deputy_remarks</t>
-  </si>
-  <si>
-    <t>EVENT_CREATED</t>
   </si>
   <si>
     <t>Logdate
@@ -314,6 +311,45 @@
   <si>
     <t>Log Date
 Log Time</t>
+  </si>
+  <si>
+    <t>IMPORTANT_COMMENTS</t>
+  </si>
+  <si>
+    <t>GENERAL_COMMENTS</t>
+  </si>
+  <si>
+    <t>MINOR_COMMENTS</t>
+  </si>
+  <si>
+    <t>OBSERVATION</t>
+  </si>
+  <si>
+    <t>VISITS</t>
+  </si>
+  <si>
+    <t>HW_SPECIAL_CASE</t>
+  </si>
+  <si>
+    <t>TELEPHONE_COMPLAINT</t>
+  </si>
+  <si>
+    <t>BOND_PROVIDER_CHANGE</t>
+  </si>
+  <si>
+    <t>ANNUAL_REPORTS</t>
+  </si>
+  <si>
+    <t>FINANCE_TRACKING</t>
+  </si>
+  <si>
+    <t>Finance Tracking</t>
+  </si>
+  <si>
+    <t>DEPUTY_DECEASED_DISCHARGED</t>
+  </si>
+  <si>
+    <t>PANEL</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1080,10 @@
         <v>34</v>
       </c>
       <c r="J8" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" t="s">
         <v>93</v>
-      </c>
-      <c r="K8" t="s">
-        <v>94</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>85</v>
@@ -2522,7 +2558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEA7712-2DD9-FE43-BF40-300AEE11EF42}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
@@ -2772,10 +2808,10 @@
         <v>34</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O8" s="14" t="s">
         <v>85</v>
@@ -4257,7 +4293,9 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5871,15 +5909,16 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="43.83203125" customWidth="1"/>
-    <col min="4" max="6" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="5" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5905,7 +5944,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5917,7 +5956,7 @@
         <v>47</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5929,7 +5968,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5941,7 +5980,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5953,7 +5992,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5965,7 +6004,7 @@
         <v>55</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5977,7 +6016,7 @@
         <v>57</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5989,7 +6028,7 @@
         <v>60</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6001,7 +6040,7 @@
         <v>62</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6010,10 +6049,10 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6025,7 +6064,7 @@
         <v>66</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -6037,7 +6076,7 @@
         <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
IN-1030 update note subtypes (#577)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuahawxwell/dev/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79C2BE3-66C3-EB4D-B506-1827A668B1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C9220-D9CD-2E48-8394-4D1A5D430114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30380" yWindow="4060" windowWidth="27440" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15420" yWindow="5940" windowWidth="35400" windowHeight="22480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="108">
   <si>
     <t>table_name</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>deputy_remarks</t>
-  </si>
-  <si>
-    <t>EVENT_CREATED</t>
   </si>
   <si>
     <t>Logdate
@@ -314,6 +311,45 @@
   <si>
     <t>Log Date
 Log Time</t>
+  </si>
+  <si>
+    <t>IMPORTANT_COMMENTS</t>
+  </si>
+  <si>
+    <t>GENERAL_COMMENTS</t>
+  </si>
+  <si>
+    <t>MINOR_COMMENTS</t>
+  </si>
+  <si>
+    <t>OBSERVATION</t>
+  </si>
+  <si>
+    <t>VISITS</t>
+  </si>
+  <si>
+    <t>HW_SPECIAL_CASE</t>
+  </si>
+  <si>
+    <t>TELEPHONE_COMPLAINT</t>
+  </si>
+  <si>
+    <t>BOND_PROVIDER_CHANGE</t>
+  </si>
+  <si>
+    <t>ANNUAL_REPORTS</t>
+  </si>
+  <si>
+    <t>FINANCE_TRACKING</t>
+  </si>
+  <si>
+    <t>Finance Tracking</t>
+  </si>
+  <si>
+    <t>DEPUTY_DECEASED_DISCHARGED</t>
+  </si>
+  <si>
+    <t>PANEL</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1080,10 @@
         <v>34</v>
       </c>
       <c r="J8" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" t="s">
         <v>93</v>
-      </c>
-      <c r="K8" t="s">
-        <v>94</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>85</v>
@@ -2522,7 +2558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEA7712-2DD9-FE43-BF40-300AEE11EF42}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
@@ -2772,10 +2808,10 @@
         <v>34</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O8" s="14" t="s">
         <v>85</v>
@@ -4257,7 +4293,9 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5871,15 +5909,16 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="43.83203125" customWidth="1"/>
-    <col min="4" max="6" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="5" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -5905,7 +5944,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5917,7 +5956,7 @@
         <v>47</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5929,7 +5968,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5941,7 +5980,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5953,7 +5992,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5965,7 +6004,7 @@
         <v>55</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5977,7 +6016,7 @@
         <v>57</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5989,7 +6028,7 @@
         <v>60</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6001,7 +6040,7 @@
         <v>62</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6010,10 +6049,10 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6025,7 +6064,7 @@
         <v>66</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -6037,7 +6076,7 @@
         <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
IN-1156 Set client and deputy notes to use correct assignee
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C9220-D9CD-2E48-8394-4D1A5D430114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB62CCE-200A-2B4E-9B67-455F17E324A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="5940" windowWidth="35400" windowHeight="22480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11740" yWindow="12180" windowWidth="42080" windowHeight="18740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="110">
   <si>
     <t>table_name</t>
   </si>
@@ -350,13 +350,19 @@
   </si>
   <si>
     <t>PANEL</t>
+  </si>
+  <si>
+    <t>assignee_lookup</t>
+  </si>
+  <si>
+    <t>by</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -436,6 +442,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -486,7 +498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -522,6 +534,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,9 +842,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P997"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1108,11 +1121,20 @@
       <c r="G9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="2">
-        <v>2</v>
+      <c r="H9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>109</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" s="21">
+        <v>2657</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>37</v>
@@ -2558,9 +2580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEA7712-2DD9-FE43-BF40-300AEE11EF42}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2836,12 +2858,20 @@
       <c r="G9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="M9" s="15">
-        <v>2</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>86</v>
+      <c r="H9" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" t="s">
+        <v>109</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" s="21">
+        <v>2657</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>37</v>
@@ -5909,7 +5939,7 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
IN-1156 Set client and deputy notes to use correct assignee (#582)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Remarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/OPG/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C9220-D9CD-2E48-8394-4D1A5D430114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB62CCE-200A-2B4E-9B67-455F17E324A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="5940" windowWidth="35400" windowHeight="22480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11740" yWindow="12180" windowWidth="42080" windowHeight="18740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="110">
   <si>
     <t>table_name</t>
   </si>
@@ -350,13 +350,19 @@
   </si>
   <si>
     <t>PANEL</t>
+  </si>
+  <si>
+    <t>assignee_lookup</t>
+  </si>
+  <si>
+    <t>by</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -436,6 +442,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -486,7 +498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -522,6 +534,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,9 +842,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P997"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1108,11 +1121,20 @@
       <c r="G9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="2">
-        <v>2</v>
+      <c r="H9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>109</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" s="21">
+        <v>2657</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>37</v>
@@ -2558,9 +2580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEA7712-2DD9-FE43-BF40-300AEE11EF42}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2836,12 +2858,20 @@
       <c r="G9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="M9" s="15">
-        <v>2</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>86</v>
+      <c r="H9" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" t="s">
+        <v>109</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" s="21">
+        <v>2657</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>37</v>
@@ -5909,7 +5939,7 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>